<commit_message>
Update Insert - Delegada Sobradinho
</commit_message>
<xml_diff>
--- a/data/raw/crcrs_delegados.xlsx
+++ b/data/raw/crcrs_delegados.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6ae8048197c0b0c2/repos/crcrs-delegados/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{5D6BA85E-BCFA-4830-A9DD-F3A0C31CF32C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B06B5CC-1EDF-40BB-9B58-F7635B831DF8}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{5D6BA85E-BCFA-4830-A9DD-F3A0C31CF32C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C2B2705-EA66-4BF3-A41F-C2E1F534905B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -900,9 +900,6 @@
     <t>Arroio do Tigre, Estrela Velha, Ibarama, Lagoa Bonita do Sul, Passa Sete, Segredo, Sobradinho, Tunas</t>
   </si>
   <si>
-    <t>Não consta</t>
-  </si>
-  <si>
     <t>Nova Prata, Nova Araçá, Nova Bassano, Paraí, André da Rocha, Vista Alegre do Prata, São Jorge, Guabiju, Protásio Alves</t>
   </si>
   <si>
@@ -910,6 +907,9 @@
   </si>
   <si>
     <t>Santa Cruz do Sul, Rio Pardo, Pantano Grande, Vera Cruz, Gramado Xavier, Sinimbu, Vale do Sol, Candelária, Herveiras, Encruzilhada do Sul, Amaral Ferrador</t>
+  </si>
+  <si>
+    <t>Cont. BRUNA SCOTA BERNARDES</t>
   </si>
 </sst>
 </file>
@@ -1249,7 +1249,7 @@
   <dimension ref="A1:C104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+      <selection activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1518,7 +1518,7 @@
         <v>100</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>219</v>
@@ -1848,7 +1848,7 @@
         <v>50</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>274</v>
@@ -1969,7 +1969,7 @@
         <v>61</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>260</v>
@@ -2203,7 +2203,7 @@
         <v>290</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">

</xml_diff>